<commit_message>
(add) edited inform in latex, added images and .exe for precaution
</commit_message>
<xml_diff>
--- a/Ejercicio_2/Results/TABLA DE RESULTADOS.xlsx
+++ b/Ejercicio_2/Results/TABLA DE RESULTADOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jesus\UNSA\Maestria\Cursos\AlgoritmosYEstructurasdeDatos\MaestriaAyEDGrupo04\Ejercicio_2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6857D2DE-02FC-4FAB-B495-77C0AED839F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248311B2-DA1A-4B67-8200-F2DBB5D6BF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32535" yWindow="705" windowWidth="20910" windowHeight="15240" xr2:uid="{360A48B5-1298-439A-8EB2-79CEDFDDB540}"/>
+    <workbookView xWindow="32535" yWindow="705" windowWidth="20910" windowHeight="15240" activeTab="2" xr2:uid="{360A48B5-1298-439A-8EB2-79CEDFDDB540}"/>
   </bookViews>
   <sheets>
     <sheet name="RESUME" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>PRUEBAS CON GRAFOS COMPLETOS</t>
   </si>
@@ -38,19 +38,29 @@
     <t>ACO</t>
   </si>
   <si>
-    <t>INTENTOS</t>
+    <t>PROMEDIO</t>
   </si>
   <si>
-    <t>PROMEDIO</t>
+    <t>BRUTE FORCE</t>
+  </si>
+  <si>
+    <t>DATA SIZE/ ITERATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -65,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,12 +83,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEFFF195-FAC8-43E8-94D5-0311F9D4BA99}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -552,304 +593,317 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A3" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="E2" s="6">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="B3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="5">
+        <f>AVERAGE(B3:F3)</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>1E-3</v>
-      </c>
-      <c r="C3">
+      <c r="B4" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="C4" s="5">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>2E-3</v>
-      </c>
-      <c r="E3">
-        <v>1E-3</v>
-      </c>
-      <c r="F3">
-        <v>1E-3</v>
-      </c>
-      <c r="G3">
-        <f>AVERAGE(B3:F3)</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1E-3</v>
-      </c>
-      <c r="C4">
+      <c r="D4" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>1E-3</v>
-      </c>
-      <c r="E4">
-        <v>1E-3</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <f t="shared" ref="G4:G13" si="0">AVERAGE(B4:F4)</f>
         <v>6.0000000000000006E-4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>1E-3</v>
-      </c>
-      <c r="D5">
-        <v>1E-3</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="E5" s="5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>1E-3</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>6.0000000000000006E-4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="5">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>1E-3</v>
-      </c>
-      <c r="C6">
-        <v>1E-3</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>1E-3</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>6.0000000000000006E-4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>1E-3</v>
-      </c>
-      <c r="C7">
-        <v>1E-3</v>
-      </c>
-      <c r="D7">
-        <v>1E-3</v>
-      </c>
-      <c r="E7">
+      <c r="B7" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="E7" s="5">
         <v>2E-3</v>
       </c>
-      <c r="F7">
-        <v>1E-3</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>1.2000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>5.7999999999999996E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>4.7E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>4.7E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>5.1400000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="5">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>0.47699999999999998</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>0.51</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>0.47799999999999998</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>0.47699999999999998</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>0.47699999999999998</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>0.4837999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="5">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>5.5250000000000004</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>5.5110000000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>5.6029999999999998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>5.5270000000000001</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>5.524</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>5.5380000000000011</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="5">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>71.518000000000001</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>67.903999999999996</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>67.902000000000001</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>68.891000000000005</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>70.281000000000006</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>69.299200000000013</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="5">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>916.42100000000005</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>914.37099999999998</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>956.83799999999997</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>891.3569</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <v>882.21400000000006</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>912.24018000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -857,327 +911,320 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF3AD19-9EFE-41A1-898F-0A1F254ECEDB}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="E2" s="6">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>1E-3</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>1E-3</v>
-      </c>
-      <c r="F3">
-        <v>1E-3</v>
-      </c>
-      <c r="G3">
+      <c r="E3" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="4">
         <f>AVERAGE(B3:F3)</f>
         <v>6.0000000000000006E-4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="5">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>1E-3</v>
-      </c>
-      <c r="C4">
-        <v>1E-3</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>1E-3</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F4" s="4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <f t="shared" ref="G4:G13" si="0">AVERAGE(B4:F4)</f>
         <v>6.0000000000000006E-4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>1E-3</v>
-      </c>
-      <c r="C5">
-        <v>1E-3</v>
-      </c>
-      <c r="D5">
-        <v>1E-3</v>
-      </c>
-      <c r="E5">
-        <v>1E-3</v>
-      </c>
-      <c r="F5">
-        <v>1E-3</v>
-      </c>
-      <c r="G5">
+      <c r="B5" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="5">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>1E-3</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="C6" s="4">
         <v>2E-3</v>
       </c>
-      <c r="D6">
-        <v>1E-3</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="E6" s="4">
         <v>2E-3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>2E-3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>2E-3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>2E-3</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>2.6000000000000003E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>3.8E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="5">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>6.8000000000000005E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="5">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="4">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>8.8000000000000005E-3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="5">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>1.1199999999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="5">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>1.3800000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C14">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="D14">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="E14">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F14">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>